<commit_message>
browser tab added in the sheet
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="channel" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,13 +13,14 @@
     <sheet name="exercise" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="video" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="exam" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="browser" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>ec756d9428c64bdb909158326108464f</t>
   </si>
@@ -94,6 +95,30 @@
   </si>
   <si>
     <t>Exam1</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>Browser </t>
+  </si>
+  <si>
+    <t>name in A1</t>
+  </si>
+  <si>
+    <t>Chrome browser</t>
+  </si>
+  <si>
+    <t>Firefox browser </t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>Internet Explorer</t>
+  </si>
+  <si>
+    <t>ie</t>
   </si>
 </sst>
 </file>
@@ -103,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -124,11 +149,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,16 +193,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -491,7 +507,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -507,8 +523,73 @@
       <c r="B1" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>